<commit_message>
Add new posts to posts.xlsx
</commit_message>
<xml_diff>
--- a/posts.xlsx
+++ b/posts.xlsx
@@ -1,37 +1,394 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10928"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yas/bluesky-bot/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EB2F79D-BC02-4D47-A3FA-03B143E470FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>image_path</t>
+  </si>
+  <si>
+    <t>hashtags</t>
+  </si>
+  <si>
+    <t>images/image1.png</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>アラビア語,test,bot</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">test text. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="178"/>
+      </rPr>
+      <t>مرحبا</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="178"/>
+      </rPr>
+      <t>يا</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="178"/>
+      </rPr>
+      <t>رفاق</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+改行
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="178"/>
+      </rPr>
+      <t>اللغة</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="178"/>
+      </rPr>
+      <t>العربية</t>
+    </r>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>images/image2.png</t>
+  </si>
+  <si>
+    <t>images/image3.png</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">2test text. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="178"/>
+      </rPr>
+      <t>مرحبا</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="178"/>
+      </rPr>
+      <t>يا</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="178"/>
+      </rPr>
+      <t>رفاق</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+改行
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="178"/>
+      </rPr>
+      <t>اللغة</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="178"/>
+      </rPr>
+      <t>العربية</t>
+    </r>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">3test 3text. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="178"/>
+      </rPr>
+      <t>مرحبا</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="178"/>
+      </rPr>
+      <t>يا</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="178"/>
+      </rPr>
+      <t>رفاق</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+改行3
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="178"/>
+      </rPr>
+      <t>اللغة</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="178"/>
+      </rPr>
+      <t>العربية</t>
+    </r>
+    <phoneticPr fontId="2"/>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4">
     <font>
-      <name val="Calibri"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="ＭＳ Ｐゴシック"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="2"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <sz val="6"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="178"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -46,93 +403,46 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="標準" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -420,37 +730,64 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <cols>
+    <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>text</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>image_path</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>hashtags</t>
-        </is>
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="75">
+      <c r="A2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="75">
+      <c r="A3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="90">
+      <c r="A4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
new posts data and images
</commit_message>
<xml_diff>
--- a/posts.xlsx
+++ b/posts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yas/bluesky-bot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFC199E9-E102-0F42-93ED-D41A865E1F0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7446240-3977-8E42-BE87-DD918F1FE7E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1783" uniqueCount="1672">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1935" uniqueCount="1824">
   <si>
     <t>text</t>
   </si>
@@ -8739,6 +8739,462 @@
   <si>
     <t xml:space="preserve">（コピー用
 0001 </t>
+  </si>
+  <si>
+    <t>images/これからアラビア文字を勉強するっていう_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/アラビア文字表_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/数字利用音訳_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/アラビア文字の字数_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「ワーウ」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「ヌーーン！！」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「タアーッ！！！」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「メリーさんのラム」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「運命」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「檻」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「口髭」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「故郷」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「ペン」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/アインの字_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「紋章」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「夢」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「忍耐」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「太陽」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「静寂／沈黙／無言」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「思い込み」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「海」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「面」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「剣」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「家」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「電球」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「心」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「真実／権利」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「一回生、四回生、卒業生」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「アート」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「猫」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「塩と砂糖」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「波」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/文字をつなげる練習_img1.jpg,images/文字をつなげる練習_img2.jpg</t>
+  </si>
+  <si>
+    <t>images/ヤーの字_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「本」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「美」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「蜘蛛」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「舌」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「宝石」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「風邪」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「時間」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「空白／空間」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「静まり」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「悪魔／サタン」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「クジラ」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「平和」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「建物」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「日の出」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「椅子」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「トゥート」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「お茶」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/バーの繋がり方_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「空いている文字を埋めましょう」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「自由」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「子猫」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「ザー、アイン、ガイン、ファー」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「きらめき」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「ガイン」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「アングル」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「物語」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「オリーブ」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「シュガー」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「ザ」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「文化」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「信頼」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「女性たち」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「三日月」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「コーヒー」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/アリフの文字_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「紙とペン」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「鏡」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「じゃんけん」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「蝶」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「いのち」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「アイデア」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「星」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/アラビア文字の繋ぎ方早見表_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/趣味_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「八月」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「八」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「ライオン」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「NARUTOシリーズ　印の結び方」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「水・火・地・空」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「六」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「グール」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「希望」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「清く正しく美しく」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「芸術」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「技／スキル」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「アラビア文字」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「力／強さ」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「経験」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「Al Ra'i」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/英語話者にとって難しい言語_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「スイカ」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「UAE」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「水」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「警察」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「速さ／スピード」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「情熱」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「助けて！」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「ロケット」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「アカデミー」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「装飾」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「パレスチナ」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「シリア」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「日本語」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「中国語」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「レバノン」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「トルコ」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「カイロ」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「アディダス」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「コカコーラ・ゼロ」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「タイド」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「SUBWAY」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「NIKE」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「ハーゲンダッツ」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「ウォルト・ディズニー」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「ポケモンGO」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「ペプシコーラ」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「キングコング」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「カンフー」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「パプリカ」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「坊っちゃん」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「一休さん」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「全身タイツ」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「ハム太郎」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「Q&amp;A 質問と回答」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「長身だ／長い」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「小さい」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「古い→新しい」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「健全なり」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「頑固だ／粘り強い」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「クーフィー体」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「忘却」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「ナマケモノ」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「プリングルズ　オリジナル味」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「朝食」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「簡単ですよ」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「壮麗」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「最強」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「両手」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「ニュース」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「星々」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「↑夢　↓現実」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/ディズニー映画_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「重大発表」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「速報」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「新しい一日」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「一人きりの旅人」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「メリークリスマス」_img1.jpg</t>
+  </si>
+  <si>
+    <t>images/「イードおめでとう」ハッピー・イード_img1.jpg,images/「イードおめでとう」ハッピー・イード_img2.jpg</t>
   </si>
 </sst>
 </file>
@@ -9122,7 +9578,7 @@
   <dimension ref="A1:C891"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C891"/>
+      <selection activeCell="A2" sqref="A2:C890"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -9147,6 +9603,9 @@
       <c r="A2" s="4" t="s">
         <v>782</v>
       </c>
+      <c r="B2" t="s">
+        <v>1672</v>
+      </c>
       <c r="C2" t="s">
         <v>3</v>
       </c>
@@ -9155,6 +9614,9 @@
       <c r="A3" s="4" t="s">
         <v>783</v>
       </c>
+      <c r="B3" t="s">
+        <v>1673</v>
+      </c>
       <c r="C3" t="s">
         <v>4</v>
       </c>
@@ -9163,6 +9625,9 @@
       <c r="A4" s="4" t="s">
         <v>784</v>
       </c>
+      <c r="B4" t="s">
+        <v>1674</v>
+      </c>
       <c r="C4" t="s">
         <v>5</v>
       </c>
@@ -9171,6 +9636,9 @@
       <c r="A5" s="4" t="s">
         <v>785</v>
       </c>
+      <c r="B5" t="s">
+        <v>1675</v>
+      </c>
       <c r="C5" t="s">
         <v>6</v>
       </c>
@@ -9179,6 +9647,9 @@
       <c r="A6" s="4" t="s">
         <v>786</v>
       </c>
+      <c r="B6" t="s">
+        <v>1676</v>
+      </c>
       <c r="C6" t="s">
         <v>7</v>
       </c>
@@ -9187,6 +9658,9 @@
       <c r="A7" s="4" t="s">
         <v>787</v>
       </c>
+      <c r="B7" t="s">
+        <v>1677</v>
+      </c>
       <c r="C7" t="s">
         <v>8</v>
       </c>
@@ -9195,6 +9669,9 @@
       <c r="A8" s="4" t="s">
         <v>788</v>
       </c>
+      <c r="B8" t="s">
+        <v>1678</v>
+      </c>
       <c r="C8" t="s">
         <v>9</v>
       </c>
@@ -9203,6 +9680,9 @@
       <c r="A9" s="4" t="s">
         <v>789</v>
       </c>
+      <c r="B9" t="s">
+        <v>1679</v>
+      </c>
       <c r="C9" t="s">
         <v>10</v>
       </c>
@@ -9211,6 +9691,9 @@
       <c r="A10" s="4" t="s">
         <v>790</v>
       </c>
+      <c r="B10" t="s">
+        <v>1680</v>
+      </c>
       <c r="C10" t="s">
         <v>11</v>
       </c>
@@ -9219,6 +9702,9 @@
       <c r="A11" s="4" t="s">
         <v>791</v>
       </c>
+      <c r="B11" t="s">
+        <v>1681</v>
+      </c>
       <c r="C11" t="s">
         <v>12</v>
       </c>
@@ -9227,6 +9713,9 @@
       <c r="A12" s="4" t="s">
         <v>792</v>
       </c>
+      <c r="B12" t="s">
+        <v>1682</v>
+      </c>
       <c r="C12" t="s">
         <v>13</v>
       </c>
@@ -9235,6 +9724,9 @@
       <c r="A13" s="4" t="s">
         <v>793</v>
       </c>
+      <c r="B13" t="s">
+        <v>1683</v>
+      </c>
       <c r="C13" t="s">
         <v>11</v>
       </c>
@@ -9243,6 +9735,9 @@
       <c r="A14" s="4" t="s">
         <v>794</v>
       </c>
+      <c r="B14" t="s">
+        <v>1684</v>
+      </c>
       <c r="C14" t="s">
         <v>14</v>
       </c>
@@ -9251,6 +9746,9 @@
       <c r="A15" s="4" t="s">
         <v>795</v>
       </c>
+      <c r="B15" t="s">
+        <v>1685</v>
+      </c>
       <c r="C15" t="s">
         <v>15</v>
       </c>
@@ -9259,6 +9757,9 @@
       <c r="A16" s="4" t="s">
         <v>796</v>
       </c>
+      <c r="B16" t="s">
+        <v>1686</v>
+      </c>
       <c r="C16" t="s">
         <v>16</v>
       </c>
@@ -9267,6 +9768,9 @@
       <c r="A17" s="4" t="s">
         <v>797</v>
       </c>
+      <c r="B17" t="s">
+        <v>1687</v>
+      </c>
       <c r="C17" t="s">
         <v>17</v>
       </c>
@@ -9275,6 +9779,9 @@
       <c r="A18" s="4" t="s">
         <v>798</v>
       </c>
+      <c r="B18" t="s">
+        <v>1688</v>
+      </c>
       <c r="C18" t="s">
         <v>18</v>
       </c>
@@ -9283,6 +9790,9 @@
       <c r="A19" s="4" t="s">
         <v>799</v>
       </c>
+      <c r="B19" t="s">
+        <v>1689</v>
+      </c>
       <c r="C19" t="s">
         <v>19</v>
       </c>
@@ -9291,6 +9801,9 @@
       <c r="A20" s="4" t="s">
         <v>800</v>
       </c>
+      <c r="B20" t="s">
+        <v>1690</v>
+      </c>
       <c r="C20" t="s">
         <v>20</v>
       </c>
@@ -9299,6 +9812,9 @@
       <c r="A21" s="4" t="s">
         <v>801</v>
       </c>
+      <c r="B21" t="s">
+        <v>1691</v>
+      </c>
       <c r="C21" t="s">
         <v>21</v>
       </c>
@@ -9307,6 +9823,9 @@
       <c r="A22" s="4" t="s">
         <v>802</v>
       </c>
+      <c r="B22" t="s">
+        <v>1692</v>
+      </c>
       <c r="C22" t="s">
         <v>11</v>
       </c>
@@ -9315,6 +9834,9 @@
       <c r="A23" s="4" t="s">
         <v>803</v>
       </c>
+      <c r="B23" t="s">
+        <v>1693</v>
+      </c>
       <c r="C23" t="s">
         <v>22</v>
       </c>
@@ -9331,6 +9853,9 @@
       <c r="A25" s="4" t="s">
         <v>805</v>
       </c>
+      <c r="B25" t="s">
+        <v>1694</v>
+      </c>
       <c r="C25" t="s">
         <v>24</v>
       </c>
@@ -9347,6 +9872,9 @@
       <c r="A27" s="4" t="s">
         <v>807</v>
       </c>
+      <c r="B27" t="s">
+        <v>1695</v>
+      </c>
       <c r="C27" t="s">
         <v>26</v>
       </c>
@@ -9355,6 +9883,9 @@
       <c r="A28" s="4" t="s">
         <v>808</v>
       </c>
+      <c r="B28" t="s">
+        <v>1696</v>
+      </c>
       <c r="C28" t="s">
         <v>27</v>
       </c>
@@ -9371,6 +9902,9 @@
       <c r="A30" s="4" t="s">
         <v>810</v>
       </c>
+      <c r="B30" t="s">
+        <v>1697</v>
+      </c>
       <c r="C30" t="s">
         <v>11</v>
       </c>
@@ -9379,6 +9913,9 @@
       <c r="A31" s="4" t="s">
         <v>811</v>
       </c>
+      <c r="B31" t="s">
+        <v>1698</v>
+      </c>
       <c r="C31" t="s">
         <v>29</v>
       </c>
@@ -9387,6 +9924,9 @@
       <c r="A32" s="4" t="s">
         <v>812</v>
       </c>
+      <c r="B32" t="s">
+        <v>1699</v>
+      </c>
       <c r="C32" t="s">
         <v>30</v>
       </c>
@@ -9395,6 +9935,9 @@
       <c r="A33" s="4" t="s">
         <v>813</v>
       </c>
+      <c r="B33" t="s">
+        <v>1700</v>
+      </c>
       <c r="C33" t="s">
         <v>31</v>
       </c>
@@ -9403,6 +9946,9 @@
       <c r="A34" s="4" t="s">
         <v>814</v>
       </c>
+      <c r="B34" t="s">
+        <v>1701</v>
+      </c>
       <c r="C34" t="s">
         <v>32</v>
       </c>
@@ -9411,6 +9957,9 @@
       <c r="A35" s="4" t="s">
         <v>815</v>
       </c>
+      <c r="B35" t="s">
+        <v>1702</v>
+      </c>
       <c r="C35" t="s">
         <v>33</v>
       </c>
@@ -9427,6 +9976,9 @@
       <c r="A37" s="4" t="s">
         <v>817</v>
       </c>
+      <c r="B37" t="s">
+        <v>1703</v>
+      </c>
       <c r="C37" t="s">
         <v>35</v>
       </c>
@@ -9435,6 +9987,9 @@
       <c r="A38" s="4" t="s">
         <v>818</v>
       </c>
+      <c r="B38" t="s">
+        <v>1704</v>
+      </c>
       <c r="C38" t="s">
         <v>36</v>
       </c>
@@ -9443,6 +9998,9 @@
       <c r="A39" s="4" t="s">
         <v>819</v>
       </c>
+      <c r="B39" t="s">
+        <v>1705</v>
+      </c>
       <c r="C39" t="s">
         <v>37</v>
       </c>
@@ -9451,6 +10009,9 @@
       <c r="A40" s="4" t="s">
         <v>820</v>
       </c>
+      <c r="B40" t="s">
+        <v>1706</v>
+      </c>
       <c r="C40" t="s">
         <v>26</v>
       </c>
@@ -9459,6 +10020,9 @@
       <c r="A41" s="4" t="s">
         <v>821</v>
       </c>
+      <c r="B41" t="s">
+        <v>1707</v>
+      </c>
       <c r="C41" t="s">
         <v>38</v>
       </c>
@@ -9467,6 +10031,9 @@
       <c r="A42" s="4" t="s">
         <v>822</v>
       </c>
+      <c r="B42" t="s">
+        <v>1708</v>
+      </c>
       <c r="C42" t="s">
         <v>39</v>
       </c>
@@ -9475,6 +10042,9 @@
       <c r="A43" s="4" t="s">
         <v>823</v>
       </c>
+      <c r="B43" t="s">
+        <v>1709</v>
+      </c>
       <c r="C43" t="s">
         <v>40</v>
       </c>
@@ -9507,6 +10077,9 @@
       <c r="A47" s="4" t="s">
         <v>827</v>
       </c>
+      <c r="B47" t="s">
+        <v>1710</v>
+      </c>
       <c r="C47" t="s">
         <v>44</v>
       </c>
@@ -9523,6 +10096,9 @@
       <c r="A49" s="4" t="s">
         <v>829</v>
       </c>
+      <c r="B49" t="s">
+        <v>1711</v>
+      </c>
       <c r="C49" t="s">
         <v>46</v>
       </c>
@@ -9531,6 +10107,9 @@
       <c r="A50" s="4" t="s">
         <v>830</v>
       </c>
+      <c r="B50" t="s">
+        <v>1712</v>
+      </c>
       <c r="C50" t="s">
         <v>47</v>
       </c>
@@ -9539,6 +10118,9 @@
       <c r="A51" s="4" t="s">
         <v>831</v>
       </c>
+      <c r="B51" t="s">
+        <v>1713</v>
+      </c>
       <c r="C51" t="s">
         <v>48</v>
       </c>
@@ -9547,6 +10129,9 @@
       <c r="A52" s="4" t="s">
         <v>832</v>
       </c>
+      <c r="B52" t="s">
+        <v>1714</v>
+      </c>
       <c r="C52" t="s">
         <v>49</v>
       </c>
@@ -9555,6 +10140,9 @@
       <c r="A53" s="4" t="s">
         <v>833</v>
       </c>
+      <c r="B53" t="s">
+        <v>1715</v>
+      </c>
       <c r="C53" t="s">
         <v>32</v>
       </c>
@@ -9563,6 +10151,9 @@
       <c r="A54" s="4" t="s">
         <v>834</v>
       </c>
+      <c r="B54" t="s">
+        <v>1716</v>
+      </c>
       <c r="C54" t="s">
         <v>32</v>
       </c>
@@ -9571,6 +10162,9 @@
       <c r="A55" s="4" t="s">
         <v>835</v>
       </c>
+      <c r="B55" t="s">
+        <v>1717</v>
+      </c>
       <c r="C55" t="s">
         <v>50</v>
       </c>
@@ -9579,6 +10173,9 @@
       <c r="A56" s="4" t="s">
         <v>836</v>
       </c>
+      <c r="B56" t="s">
+        <v>1718</v>
+      </c>
       <c r="C56" t="s">
         <v>31</v>
       </c>
@@ -9587,6 +10184,9 @@
       <c r="A57" s="4" t="s">
         <v>837</v>
       </c>
+      <c r="B57" t="s">
+        <v>1719</v>
+      </c>
       <c r="C57" t="s">
         <v>51</v>
       </c>
@@ -9595,6 +10195,9 @@
       <c r="A58" s="4" t="s">
         <v>838</v>
       </c>
+      <c r="B58" t="s">
+        <v>1720</v>
+      </c>
       <c r="C58" t="s">
         <v>52</v>
       </c>
@@ -9603,6 +10206,9 @@
       <c r="A59" s="4" t="s">
         <v>839</v>
       </c>
+      <c r="B59" t="s">
+        <v>1721</v>
+      </c>
       <c r="C59" t="s">
         <v>32</v>
       </c>
@@ -9611,6 +10217,9 @@
       <c r="A60" s="4" t="s">
         <v>840</v>
       </c>
+      <c r="B60" t="s">
+        <v>1722</v>
+      </c>
       <c r="C60" t="s">
         <v>24</v>
       </c>
@@ -9627,6 +10236,9 @@
       <c r="A62" s="4" t="s">
         <v>842</v>
       </c>
+      <c r="B62" t="s">
+        <v>1723</v>
+      </c>
       <c r="C62" t="s">
         <v>54</v>
       </c>
@@ -9651,6 +10263,9 @@
       <c r="A65" s="4" t="s">
         <v>845</v>
       </c>
+      <c r="B65" t="s">
+        <v>1724</v>
+      </c>
       <c r="C65" t="s">
         <v>32</v>
       </c>
@@ -9659,6 +10274,9 @@
       <c r="A66" s="4" t="s">
         <v>846</v>
       </c>
+      <c r="B66" t="s">
+        <v>1725</v>
+      </c>
       <c r="C66" t="s">
         <v>56</v>
       </c>
@@ -9667,6 +10285,9 @@
       <c r="A67" s="4" t="s">
         <v>847</v>
       </c>
+      <c r="B67" t="s">
+        <v>1726</v>
+      </c>
       <c r="C67" t="s">
         <v>57</v>
       </c>
@@ -9699,6 +10320,9 @@
       <c r="A71" s="4" t="s">
         <v>851</v>
       </c>
+      <c r="B71" t="s">
+        <v>1727</v>
+      </c>
       <c r="C71" t="s">
         <v>60</v>
       </c>
@@ -9707,6 +10331,9 @@
       <c r="A72" s="4" t="s">
         <v>852</v>
       </c>
+      <c r="B72" t="s">
+        <v>1728</v>
+      </c>
       <c r="C72" t="s">
         <v>61</v>
       </c>
@@ -9715,6 +10342,9 @@
       <c r="A73" s="4" t="s">
         <v>853</v>
       </c>
+      <c r="B73" t="s">
+        <v>1729</v>
+      </c>
       <c r="C73" t="s">
         <v>55</v>
       </c>
@@ -9723,6 +10353,9 @@
       <c r="A74" s="4" t="s">
         <v>854</v>
       </c>
+      <c r="B74" t="s">
+        <v>1730</v>
+      </c>
       <c r="C74" t="s">
         <v>62</v>
       </c>
@@ -9755,6 +10388,9 @@
       <c r="A78" s="4" t="s">
         <v>858</v>
       </c>
+      <c r="B78" t="s">
+        <v>1731</v>
+      </c>
       <c r="C78" t="s">
         <v>66</v>
       </c>
@@ -9771,6 +10407,9 @@
       <c r="A80" s="4" t="s">
         <v>860</v>
       </c>
+      <c r="B80" t="s">
+        <v>1732</v>
+      </c>
       <c r="C80" t="s">
         <v>67</v>
       </c>
@@ -9787,6 +10426,9 @@
       <c r="A82" s="4" t="s">
         <v>862</v>
       </c>
+      <c r="B82" t="s">
+        <v>1733</v>
+      </c>
       <c r="C82" t="s">
         <v>69</v>
       </c>
@@ -9795,6 +10437,9 @@
       <c r="A83" s="4" t="s">
         <v>863</v>
       </c>
+      <c r="B83" t="s">
+        <v>1734</v>
+      </c>
       <c r="C83" t="s">
         <v>70</v>
       </c>
@@ -9803,6 +10448,9 @@
       <c r="A84" s="4" t="s">
         <v>864</v>
       </c>
+      <c r="B84" t="s">
+        <v>1735</v>
+      </c>
       <c r="C84" t="s">
         <v>71</v>
       </c>
@@ -9811,6 +10459,9 @@
       <c r="A85" s="4" t="s">
         <v>865</v>
       </c>
+      <c r="B85" t="s">
+        <v>1736</v>
+      </c>
       <c r="C85" t="s">
         <v>72</v>
       </c>
@@ -9827,6 +10478,9 @@
       <c r="A87" s="4" t="s">
         <v>867</v>
       </c>
+      <c r="B87" t="s">
+        <v>1737</v>
+      </c>
       <c r="C87" t="s">
         <v>74</v>
       </c>
@@ -9843,6 +10497,9 @@
       <c r="A89" s="4" t="s">
         <v>869</v>
       </c>
+      <c r="B89" t="s">
+        <v>1738</v>
+      </c>
       <c r="C89" t="s">
         <v>76</v>
       </c>
@@ -9851,6 +10508,9 @@
       <c r="A90" s="4" t="s">
         <v>870</v>
       </c>
+      <c r="B90" t="s">
+        <v>1739</v>
+      </c>
       <c r="C90" t="s">
         <v>77</v>
       </c>
@@ -9859,6 +10519,9 @@
       <c r="A91" s="4" t="s">
         <v>871</v>
       </c>
+      <c r="B91" t="s">
+        <v>1740</v>
+      </c>
       <c r="C91" t="s">
         <v>42</v>
       </c>
@@ -9883,6 +10546,9 @@
       <c r="A94" s="4" t="s">
         <v>874</v>
       </c>
+      <c r="B94" t="s">
+        <v>1741</v>
+      </c>
       <c r="C94" t="s">
         <v>79</v>
       </c>
@@ -9891,6 +10557,9 @@
       <c r="A95" s="4" t="s">
         <v>875</v>
       </c>
+      <c r="B95" t="s">
+        <v>1742</v>
+      </c>
       <c r="C95" t="s">
         <v>80</v>
       </c>
@@ -9899,6 +10568,9 @@
       <c r="A96" s="4" t="s">
         <v>876</v>
       </c>
+      <c r="B96" t="s">
+        <v>1743</v>
+      </c>
       <c r="C96" t="s">
         <v>81</v>
       </c>
@@ -9907,6 +10579,9 @@
       <c r="A97" s="4" t="s">
         <v>877</v>
       </c>
+      <c r="B97" t="s">
+        <v>1744</v>
+      </c>
       <c r="C97" t="s">
         <v>82</v>
       </c>
@@ -9915,6 +10590,9 @@
       <c r="A98" s="4" t="s">
         <v>878</v>
       </c>
+      <c r="B98" t="s">
+        <v>1745</v>
+      </c>
       <c r="C98" t="s">
         <v>83</v>
       </c>
@@ -9923,6 +10601,9 @@
       <c r="A99" s="4" t="s">
         <v>879</v>
       </c>
+      <c r="B99" t="s">
+        <v>1746</v>
+      </c>
       <c r="C99" t="s">
         <v>84</v>
       </c>
@@ -9931,6 +10612,9 @@
       <c r="A100" s="4" t="s">
         <v>880</v>
       </c>
+      <c r="B100" t="s">
+        <v>1747</v>
+      </c>
       <c r="C100" t="s">
         <v>85</v>
       </c>
@@ -9939,6 +10623,9 @@
       <c r="A101" s="4" t="s">
         <v>881</v>
       </c>
+      <c r="B101" t="s">
+        <v>1748</v>
+      </c>
       <c r="C101" t="s">
         <v>86</v>
       </c>
@@ -9955,6 +10642,9 @@
       <c r="A103" s="4" t="s">
         <v>883</v>
       </c>
+      <c r="B103" t="s">
+        <v>1749</v>
+      </c>
       <c r="C103" t="s">
         <v>88</v>
       </c>
@@ -9963,6 +10653,9 @@
       <c r="A104" s="4" t="s">
         <v>884</v>
       </c>
+      <c r="B104" t="s">
+        <v>1750</v>
+      </c>
       <c r="C104" t="s">
         <v>89</v>
       </c>
@@ -9971,6 +10664,9 @@
       <c r="A105" s="4" t="s">
         <v>885</v>
       </c>
+      <c r="B105" t="s">
+        <v>1751</v>
+      </c>
       <c r="C105" t="s">
         <v>90</v>
       </c>
@@ -9979,6 +10675,9 @@
       <c r="A106" s="4" t="s">
         <v>886</v>
       </c>
+      <c r="B106" t="s">
+        <v>1752</v>
+      </c>
       <c r="C106" t="s">
         <v>32</v>
       </c>
@@ -9987,6 +10686,9 @@
       <c r="A107" s="4" t="s">
         <v>887</v>
       </c>
+      <c r="B107" t="s">
+        <v>1753</v>
+      </c>
       <c r="C107" t="s">
         <v>91</v>
       </c>
@@ -9995,6 +10697,9 @@
       <c r="A108" s="4" t="s">
         <v>888</v>
       </c>
+      <c r="B108" t="s">
+        <v>1754</v>
+      </c>
       <c r="C108" t="s">
         <v>92</v>
       </c>
@@ -10003,6 +10708,9 @@
       <c r="A109" s="4" t="s">
         <v>889</v>
       </c>
+      <c r="B109" t="s">
+        <v>1755</v>
+      </c>
       <c r="C109" t="s">
         <v>42</v>
       </c>
@@ -10019,6 +10727,9 @@
       <c r="A111" s="4" t="s">
         <v>891</v>
       </c>
+      <c r="B111" t="s">
+        <v>1756</v>
+      </c>
       <c r="C111" t="s">
         <v>94</v>
       </c>
@@ -10035,6 +10746,9 @@
       <c r="A113" s="4" t="s">
         <v>893</v>
       </c>
+      <c r="B113" t="s">
+        <v>1757</v>
+      </c>
       <c r="C113" t="s">
         <v>96</v>
       </c>
@@ -10051,6 +10765,9 @@
       <c r="A115" s="4" t="s">
         <v>895</v>
       </c>
+      <c r="B115" t="s">
+        <v>1758</v>
+      </c>
       <c r="C115" t="s">
         <v>98</v>
       </c>
@@ -10059,6 +10776,9 @@
       <c r="A116" s="4" t="s">
         <v>896</v>
       </c>
+      <c r="B116" t="s">
+        <v>1759</v>
+      </c>
       <c r="C116" t="s">
         <v>99</v>
       </c>
@@ -10075,6 +10795,9 @@
       <c r="A118" s="4" t="s">
         <v>898</v>
       </c>
+      <c r="B118" t="s">
+        <v>1760</v>
+      </c>
       <c r="C118" t="s">
         <v>95</v>
       </c>
@@ -10083,6 +10806,9 @@
       <c r="A119" s="4" t="s">
         <v>899</v>
       </c>
+      <c r="B119" t="s">
+        <v>1761</v>
+      </c>
       <c r="C119" t="s">
         <v>101</v>
       </c>
@@ -10091,6 +10817,9 @@
       <c r="A120" s="4" t="s">
         <v>900</v>
       </c>
+      <c r="B120" t="s">
+        <v>1762</v>
+      </c>
       <c r="C120" t="s">
         <v>95</v>
       </c>
@@ -10107,6 +10836,9 @@
       <c r="A122" s="4" t="s">
         <v>902</v>
       </c>
+      <c r="B122" t="s">
+        <v>1763</v>
+      </c>
       <c r="C122" t="s">
         <v>95</v>
       </c>
@@ -10115,6 +10847,9 @@
       <c r="A123" s="4" t="s">
         <v>903</v>
       </c>
+      <c r="B123" t="s">
+        <v>1764</v>
+      </c>
       <c r="C123" t="s">
         <v>103</v>
       </c>
@@ -10123,6 +10858,9 @@
       <c r="A124" s="4" t="s">
         <v>904</v>
       </c>
+      <c r="B124" t="s">
+        <v>1765</v>
+      </c>
       <c r="C124" t="s">
         <v>104</v>
       </c>
@@ -10131,6 +10869,9 @@
       <c r="A125" s="4" t="s">
         <v>905</v>
       </c>
+      <c r="B125" t="s">
+        <v>1766</v>
+      </c>
       <c r="C125" t="s">
         <v>105</v>
       </c>
@@ -10139,6 +10880,9 @@
       <c r="A126" s="4" t="s">
         <v>906</v>
       </c>
+      <c r="B126" t="s">
+        <v>1767</v>
+      </c>
       <c r="C126" t="s">
         <v>106</v>
       </c>
@@ -10147,6 +10891,9 @@
       <c r="A127" s="4" t="s">
         <v>907</v>
       </c>
+      <c r="B127" t="s">
+        <v>1768</v>
+      </c>
       <c r="C127" t="s">
         <v>107</v>
       </c>
@@ -10155,6 +10902,9 @@
       <c r="A128" s="4" t="s">
         <v>908</v>
       </c>
+      <c r="B128" t="s">
+        <v>1769</v>
+      </c>
       <c r="C128" t="s">
         <v>108</v>
       </c>
@@ -10171,6 +10921,9 @@
       <c r="A130" s="4" t="s">
         <v>910</v>
       </c>
+      <c r="B130" t="s">
+        <v>1770</v>
+      </c>
       <c r="C130" t="s">
         <v>109</v>
       </c>
@@ -10187,6 +10940,9 @@
       <c r="A132" s="4" t="s">
         <v>912</v>
       </c>
+      <c r="B132" t="s">
+        <v>1771</v>
+      </c>
       <c r="C132" t="s">
         <v>110</v>
       </c>
@@ -10195,6 +10951,9 @@
       <c r="A133" s="4" t="s">
         <v>913</v>
       </c>
+      <c r="B133" t="s">
+        <v>1772</v>
+      </c>
       <c r="C133" t="s">
         <v>111</v>
       </c>
@@ -10211,6 +10970,9 @@
       <c r="A135" s="4" t="s">
         <v>915</v>
       </c>
+      <c r="B135" t="s">
+        <v>1773</v>
+      </c>
       <c r="C135" t="s">
         <v>113</v>
       </c>
@@ -10219,6 +10981,9 @@
       <c r="A136" s="4" t="s">
         <v>916</v>
       </c>
+      <c r="B136" t="s">
+        <v>1774</v>
+      </c>
       <c r="C136" t="s">
         <v>42</v>
       </c>
@@ -10227,6 +10992,9 @@
       <c r="A137" s="4" t="s">
         <v>917</v>
       </c>
+      <c r="B137" t="s">
+        <v>1775</v>
+      </c>
       <c r="C137" t="s">
         <v>114</v>
       </c>
@@ -10243,6 +11011,9 @@
       <c r="A139" s="4" t="s">
         <v>919</v>
       </c>
+      <c r="B139" t="s">
+        <v>1776</v>
+      </c>
       <c r="C139" t="s">
         <v>116</v>
       </c>
@@ -10251,6 +11022,9 @@
       <c r="A140" s="4" t="s">
         <v>920</v>
       </c>
+      <c r="B140" t="s">
+        <v>1777</v>
+      </c>
       <c r="C140" t="s">
         <v>31</v>
       </c>
@@ -10259,6 +11033,9 @@
       <c r="A141" s="4" t="s">
         <v>921</v>
       </c>
+      <c r="B141" t="s">
+        <v>1778</v>
+      </c>
       <c r="C141" t="s">
         <v>32</v>
       </c>
@@ -10267,6 +11044,9 @@
       <c r="A142" s="4" t="s">
         <v>922</v>
       </c>
+      <c r="B142" t="s">
+        <v>1779</v>
+      </c>
       <c r="C142" t="s">
         <v>117</v>
       </c>
@@ -10275,6 +11055,9 @@
       <c r="A143" s="4" t="s">
         <v>923</v>
       </c>
+      <c r="B143" t="s">
+        <v>1780</v>
+      </c>
       <c r="C143" t="s">
         <v>118</v>
       </c>
@@ -10283,6 +11066,9 @@
       <c r="A144" s="4" t="s">
         <v>924</v>
       </c>
+      <c r="B144" t="s">
+        <v>1781</v>
+      </c>
       <c r="C144" t="s">
         <v>119</v>
       </c>
@@ -10299,6 +11085,9 @@
       <c r="A146" s="4" t="s">
         <v>926</v>
       </c>
+      <c r="B146" t="s">
+        <v>1782</v>
+      </c>
       <c r="C146" t="s">
         <v>121</v>
       </c>
@@ -10323,6 +11112,9 @@
       <c r="A149" s="4" t="s">
         <v>929</v>
       </c>
+      <c r="B149" t="s">
+        <v>1783</v>
+      </c>
       <c r="C149" t="s">
         <v>124</v>
       </c>
@@ -10331,6 +11123,9 @@
       <c r="A150" s="4" t="s">
         <v>930</v>
       </c>
+      <c r="B150" t="s">
+        <v>1784</v>
+      </c>
       <c r="C150" t="s">
         <v>125</v>
       </c>
@@ -10347,6 +11142,9 @@
       <c r="A152" s="4" t="s">
         <v>932</v>
       </c>
+      <c r="B152" t="s">
+        <v>1785</v>
+      </c>
       <c r="C152" t="s">
         <v>126</v>
       </c>
@@ -10355,6 +11153,9 @@
       <c r="A153" s="4" t="s">
         <v>933</v>
       </c>
+      <c r="B153" t="s">
+        <v>1786</v>
+      </c>
       <c r="C153" t="s">
         <v>127</v>
       </c>
@@ -10363,6 +11164,9 @@
       <c r="A154" s="4" t="s">
         <v>934</v>
       </c>
+      <c r="B154" t="s">
+        <v>1787</v>
+      </c>
       <c r="C154" t="s">
         <v>128</v>
       </c>
@@ -10379,6 +11183,9 @@
       <c r="A156" s="4" t="s">
         <v>936</v>
       </c>
+      <c r="B156" t="s">
+        <v>1788</v>
+      </c>
       <c r="C156" t="s">
         <v>127</v>
       </c>
@@ -10387,6 +11194,9 @@
       <c r="A157" s="4" t="s">
         <v>937</v>
       </c>
+      <c r="B157" t="s">
+        <v>1789</v>
+      </c>
       <c r="C157" t="s">
         <v>130</v>
       </c>
@@ -10395,6 +11205,9 @@
       <c r="A158" s="4" t="s">
         <v>938</v>
       </c>
+      <c r="B158" t="s">
+        <v>1790</v>
+      </c>
       <c r="C158" t="s">
         <v>131</v>
       </c>
@@ -10403,6 +11216,9 @@
       <c r="A159" s="4" t="s">
         <v>939</v>
       </c>
+      <c r="B159" t="s">
+        <v>1791</v>
+      </c>
       <c r="C159" t="s">
         <v>132</v>
       </c>
@@ -10411,6 +11227,9 @@
       <c r="A160" s="4" t="s">
         <v>940</v>
       </c>
+      <c r="B160" t="s">
+        <v>1792</v>
+      </c>
       <c r="C160" t="s">
         <v>133</v>
       </c>
@@ -10419,6 +11238,9 @@
       <c r="A161" s="4" t="s">
         <v>941</v>
       </c>
+      <c r="B161" t="s">
+        <v>1793</v>
+      </c>
       <c r="C161" t="s">
         <v>134</v>
       </c>
@@ -10443,6 +11265,9 @@
       <c r="A164" s="4" t="s">
         <v>944</v>
       </c>
+      <c r="B164" t="s">
+        <v>1794</v>
+      </c>
       <c r="C164" t="s">
         <v>136</v>
       </c>
@@ -10451,6 +11276,9 @@
       <c r="A165" s="4" t="s">
         <v>945</v>
       </c>
+      <c r="B165" t="s">
+        <v>1795</v>
+      </c>
       <c r="C165" t="s">
         <v>137</v>
       </c>
@@ -10459,6 +11287,9 @@
       <c r="A166" s="4" t="s">
         <v>946</v>
       </c>
+      <c r="B166" t="s">
+        <v>1796</v>
+      </c>
       <c r="C166" t="s">
         <v>138</v>
       </c>
@@ -10475,6 +11306,9 @@
       <c r="A168" s="4" t="s">
         <v>948</v>
       </c>
+      <c r="B168" t="s">
+        <v>1797</v>
+      </c>
       <c r="C168" t="s">
         <v>42</v>
       </c>
@@ -10483,6 +11317,9 @@
       <c r="A169" s="4" t="s">
         <v>949</v>
       </c>
+      <c r="B169" t="s">
+        <v>1798</v>
+      </c>
       <c r="C169" t="s">
         <v>140</v>
       </c>
@@ -10491,6 +11328,9 @@
       <c r="A170" s="4" t="s">
         <v>950</v>
       </c>
+      <c r="B170" t="s">
+        <v>1799</v>
+      </c>
       <c r="C170" t="s">
         <v>141</v>
       </c>
@@ -10499,6 +11339,9 @@
       <c r="A171" s="4" t="s">
         <v>951</v>
       </c>
+      <c r="B171" t="s">
+        <v>1800</v>
+      </c>
       <c r="C171" t="s">
         <v>142</v>
       </c>
@@ -10507,6 +11350,9 @@
       <c r="A172" s="4" t="s">
         <v>952</v>
       </c>
+      <c r="B172" t="s">
+        <v>1801</v>
+      </c>
       <c r="C172" t="s">
         <v>143</v>
       </c>
@@ -10515,6 +11361,9 @@
       <c r="A173" s="4" t="s">
         <v>953</v>
       </c>
+      <c r="B173" t="s">
+        <v>1802</v>
+      </c>
       <c r="C173" t="s">
         <v>144</v>
       </c>
@@ -10523,6 +11372,9 @@
       <c r="A174" s="4" t="s">
         <v>954</v>
       </c>
+      <c r="B174" t="s">
+        <v>1803</v>
+      </c>
       <c r="C174" t="s">
         <v>145</v>
       </c>
@@ -10531,6 +11383,9 @@
       <c r="A175" s="4" t="s">
         <v>955</v>
       </c>
+      <c r="B175" t="s">
+        <v>1804</v>
+      </c>
       <c r="C175" t="s">
         <v>146</v>
       </c>
@@ -10539,6 +11394,9 @@
       <c r="A176" s="4" t="s">
         <v>956</v>
       </c>
+      <c r="B176" t="s">
+        <v>1805</v>
+      </c>
       <c r="C176" t="s">
         <v>147</v>
       </c>
@@ -10547,6 +11405,9 @@
       <c r="A177" s="4" t="s">
         <v>957</v>
       </c>
+      <c r="B177" t="s">
+        <v>1806</v>
+      </c>
       <c r="C177" t="s">
         <v>32</v>
       </c>
@@ -10555,6 +11416,9 @@
       <c r="A178" s="4" t="s">
         <v>958</v>
       </c>
+      <c r="B178" t="s">
+        <v>1807</v>
+      </c>
       <c r="C178" t="s">
         <v>148</v>
       </c>
@@ -10563,6 +11427,9 @@
       <c r="A179" s="4" t="s">
         <v>959</v>
       </c>
+      <c r="B179" t="s">
+        <v>1808</v>
+      </c>
       <c r="C179" t="s">
         <v>149</v>
       </c>
@@ -10571,6 +11438,9 @@
       <c r="A180" s="4" t="s">
         <v>960</v>
       </c>
+      <c r="B180" t="s">
+        <v>1809</v>
+      </c>
       <c r="C180" t="s">
         <v>150</v>
       </c>
@@ -10587,6 +11457,9 @@
       <c r="A182" s="4" t="s">
         <v>962</v>
       </c>
+      <c r="B182" t="s">
+        <v>1810</v>
+      </c>
       <c r="C182" t="s">
         <v>152</v>
       </c>
@@ -10595,6 +11468,9 @@
       <c r="A183" s="4" t="s">
         <v>963</v>
       </c>
+      <c r="B183" t="s">
+        <v>1811</v>
+      </c>
       <c r="C183" t="s">
         <v>153</v>
       </c>
@@ -10603,6 +11479,9 @@
       <c r="A184" s="4" t="s">
         <v>964</v>
       </c>
+      <c r="B184" t="s">
+        <v>1812</v>
+      </c>
       <c r="C184" t="s">
         <v>154</v>
       </c>
@@ -10611,6 +11490,9 @@
       <c r="A185" s="4" t="s">
         <v>965</v>
       </c>
+      <c r="B185" t="s">
+        <v>1813</v>
+      </c>
       <c r="C185" t="s">
         <v>42</v>
       </c>
@@ -10627,6 +11509,9 @@
       <c r="A187" s="4" t="s">
         <v>967</v>
       </c>
+      <c r="B187" t="s">
+        <v>1814</v>
+      </c>
       <c r="C187" t="s">
         <v>156</v>
       </c>
@@ -10643,6 +11528,9 @@
       <c r="A189" s="4" t="s">
         <v>969</v>
       </c>
+      <c r="B189" t="s">
+        <v>1815</v>
+      </c>
       <c r="C189" t="s">
         <v>157</v>
       </c>
@@ -10651,6 +11539,9 @@
       <c r="A190" s="4" t="s">
         <v>970</v>
       </c>
+      <c r="B190" t="s">
+        <v>1816</v>
+      </c>
       <c r="C190" t="s">
         <v>158</v>
       </c>
@@ -10659,6 +11550,9 @@
       <c r="A191" s="4" t="s">
         <v>971</v>
       </c>
+      <c r="B191" t="s">
+        <v>1817</v>
+      </c>
       <c r="C191" t="s">
         <v>159</v>
       </c>
@@ -10667,6 +11561,9 @@
       <c r="A192" s="4" t="s">
         <v>972</v>
       </c>
+      <c r="B192" t="s">
+        <v>1818</v>
+      </c>
       <c r="C192" t="s">
         <v>160</v>
       </c>
@@ -10675,6 +11572,9 @@
       <c r="A193" s="4" t="s">
         <v>973</v>
       </c>
+      <c r="B193" t="s">
+        <v>1819</v>
+      </c>
       <c r="C193" t="s">
         <v>120</v>
       </c>
@@ -10683,6 +11583,9 @@
       <c r="A194" s="4" t="s">
         <v>974</v>
       </c>
+      <c r="B194" t="s">
+        <v>1820</v>
+      </c>
       <c r="C194" t="s">
         <v>161</v>
       </c>
@@ -10691,6 +11594,9 @@
       <c r="A195" s="4" t="s">
         <v>975</v>
       </c>
+      <c r="B195" t="s">
+        <v>1821</v>
+      </c>
       <c r="C195" t="s">
         <v>162</v>
       </c>
@@ -10699,6 +11605,9 @@
       <c r="A196" s="4" t="s">
         <v>976</v>
       </c>
+      <c r="B196" t="s">
+        <v>1822</v>
+      </c>
       <c r="C196" t="s">
         <v>163</v>
       </c>
@@ -10706,6 +11615,9 @@
     <row r="197" spans="1:3" ht="75">
       <c r="A197" s="4" t="s">
         <v>977</v>
+      </c>
+      <c r="B197" t="s">
+        <v>1823</v>
       </c>
       <c r="C197" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
Update posts.xlsx after post
</commit_message>
<xml_diff>
--- a/posts.xlsx
+++ b/posts.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C888"/>
+  <dimension ref="A1:C887"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15867,23 +15867,6 @@
     <row r="874">
       <c r="A874" t="inlineStr">
         <is>
-          <t xml:space="preserve">「行くな」ماتروحش
-マトロホシ [ma-troH-Sh]
-⁦方言：「あなたは行く／去る」ティローホ ( تروح )[te-rooH]・「〜ない」( ما .. ـش )[ma--Sh]：( شـشـش )[Sh-Sh-Sh]⁩
-行く（いく）
-2411 triiq tumblr </t>
-        </is>
-      </c>
-      <c r="B874" t="inlineStr"/>
-      <c r="C874" t="inlineStr">
-        <is>
-          <t>ロゴ ,デザイン ,嵐</t>
-        </is>
-      </c>
-    </row>
-    <row r="875">
-      <c r="A875" t="inlineStr">
-        <is>
           <t xml:space="preserve">⁦「元気？」⁩شلونَك؟
 シュローナク？ [Sh-loon-ak?]
 方言。対男性。
@@ -15893,15 +15876,15 @@
 2202 出典不明 </t>
         </is>
       </c>
-      <c r="B875" t="inlineStr"/>
-      <c r="C875" t="inlineStr">
+      <c r="B874" t="inlineStr"/>
+      <c r="C874" t="inlineStr">
         <is>
           <t>洒落 ,挨拶</t>
         </is>
       </c>
     </row>
-    <row r="876">
-      <c r="A876" t="inlineStr">
+    <row r="875">
+      <c r="A875" t="inlineStr">
         <is>
           <t xml:space="preserve">「気分が良いぞう」I فيل GOOD
 アイ・フィール・グッド [ai fiyl gud]
@@ -15910,15 +15893,15 @@
 2308 出典不明 </t>
         </is>
       </c>
-      <c r="B876" t="inlineStr"/>
-      <c r="C876" t="inlineStr">
+      <c r="B875" t="inlineStr"/>
+      <c r="C875" t="inlineStr">
         <is>
           <t>洒落 ,和訳</t>
         </is>
       </c>
     </row>
-    <row r="877">
-      <c r="A877" t="inlineStr">
+    <row r="876">
+      <c r="A876" t="inlineStr">
         <is>
           <t xml:space="preserve">「レットイットゴー／let it go」
 ليت اِت غو
@@ -15927,15 +15910,15 @@
 2109 出典不明 </t>
         </is>
       </c>
-      <c r="B877" t="inlineStr"/>
-      <c r="C877" t="inlineStr">
+      <c r="B876" t="inlineStr"/>
+      <c r="C876" t="inlineStr">
         <is>
           <t>折衷 ,アナ雪</t>
         </is>
       </c>
     </row>
-    <row r="878">
-      <c r="A878" t="inlineStr">
+    <row r="877">
+      <c r="A877" t="inlineStr">
         <is>
           <t xml:space="preserve">「ようこそ」اهلا وسهلا
 アハラン・ワサハラン ['ahlan wa-sahlan]
@@ -15943,15 +15926,15 @@
 2106 behance Anwar Al Eissa </t>
         </is>
       </c>
-      <c r="B878" t="inlineStr"/>
-      <c r="C878" t="inlineStr">
+      <c r="B877" t="inlineStr"/>
+      <c r="C877" t="inlineStr">
         <is>
           <t>アラビア語</t>
         </is>
       </c>
     </row>
-    <row r="879">
-      <c r="A879" t="inlineStr">
+    <row r="878">
+      <c r="A878" t="inlineStr">
         <is>
           <t xml:space="preserve">「まぁ何というサプライズでしょう」
 يا لها من مفاجأة
@@ -15962,15 +15945,15 @@
 2108 neelwafurat com </t>
         </is>
       </c>
-      <c r="B879" t="inlineStr"/>
-      <c r="C879" t="inlineStr">
+      <c r="B878" t="inlineStr"/>
+      <c r="C878" t="inlineStr">
         <is>
           <t>中国語 ,学習</t>
         </is>
       </c>
     </row>
-    <row r="880">
-      <c r="A880" t="inlineStr">
+    <row r="879">
+      <c r="A879" t="inlineStr">
         <is>
           <t xml:space="preserve">「ハックション」اتشوو
 アチュー！ ['aatShuu]
@@ -15978,11 +15961,11 @@
 1811 #あらびあや </t>
         </is>
       </c>
-      <c r="B880" t="inlineStr"/>
-      <c r="C880" t="inlineStr"/>
-    </row>
-    <row r="881">
-      <c r="A881" t="inlineStr">
+      <c r="B879" t="inlineStr"/>
+      <c r="C879" t="inlineStr"/>
+    </row>
+    <row r="880">
+      <c r="A880" t="inlineStr">
         <is>
           <t xml:space="preserve">「スブハーナッラー」「アルハムドゥリッラー」「アッラーアクバル」
 سبحان الله
@@ -15993,15 +15976,15 @@
 2308 dribbble com </t>
         </is>
       </c>
-      <c r="B881" t="inlineStr"/>
-      <c r="C881" t="inlineStr">
+      <c r="B880" t="inlineStr"/>
+      <c r="C880" t="inlineStr">
         <is>
           <t>四角 ,コンパクト</t>
         </is>
       </c>
     </row>
-    <row r="882">
-      <c r="A882" t="inlineStr">
+    <row r="881">
+      <c r="A881" t="inlineStr">
         <is>
           <t xml:space="preserve">「すごく美味しい！」لذيذ جدًا
 ラズィーズ・ジッダン [laDhiiDh jiddan]
@@ -16010,15 +15993,15 @@
 2109 goodreads com </t>
         </is>
       </c>
-      <c r="B882" t="inlineStr"/>
-      <c r="C882" t="inlineStr">
+      <c r="B881" t="inlineStr"/>
+      <c r="C881" t="inlineStr">
         <is>
           <t>フレーズ ,感想</t>
         </is>
       </c>
     </row>
-    <row r="883">
-      <c r="A883" t="inlineStr">
+    <row r="882">
+      <c r="A882" t="inlineStr">
         <is>
           <t xml:space="preserve">「しとしと、雨」تك تك يا مطر
 ティクティク [tik tik yaa ma_tar]
@@ -16027,15 +16010,15 @@
 2308 出典不明 </t>
         </is>
       </c>
-      <c r="B883" t="inlineStr"/>
-      <c r="C883" t="inlineStr">
+      <c r="B882" t="inlineStr"/>
+      <c r="C882" t="inlineStr">
         <is>
           <t>天気 ,梅雨</t>
         </is>
       </c>
     </row>
-    <row r="884">
-      <c r="A884" t="inlineStr">
+    <row r="883">
+      <c r="A883" t="inlineStr">
         <is>
           <t xml:space="preserve">「さかさま」رأساً على عقب
 ラッアサン・アラー・アケブ [ra'san *alaa *aqib]
@@ -16043,15 +16026,15 @@
 2109 出典不明 </t>
         </is>
       </c>
-      <c r="B884" t="inlineStr"/>
-      <c r="C884" t="inlineStr">
+      <c r="B883" t="inlineStr"/>
+      <c r="C883" t="inlineStr">
         <is>
           <t>壁 ,上下</t>
         </is>
       </c>
     </row>
-    <row r="885">
-      <c r="A885" t="inlineStr">
+    <row r="884">
+      <c r="A884" t="inlineStr">
         <is>
           <t xml:space="preserve">「エジプトよどこへ行った」
 فينك يا مصر؟
@@ -16061,15 +16044,15 @@
 1809 shehabfawzy1.tumblr </t>
         </is>
       </c>
-      <c r="B885" t="inlineStr"/>
-      <c r="C885" t="inlineStr">
+      <c r="B884" t="inlineStr"/>
+      <c r="C884" t="inlineStr">
         <is>
           <t>ピラミッド ,歴史</t>
         </is>
       </c>
     </row>
-    <row r="886">
-      <c r="A886" t="inlineStr">
+    <row r="885">
+      <c r="A885" t="inlineStr">
         <is>
           <t xml:space="preserve">「ありがとう」شكراً
 シュクラン [Shukran]
@@ -16077,15 +16060,15 @@
 2109 出典不明 </t>
         </is>
       </c>
-      <c r="B886" t="inlineStr"/>
-      <c r="C886" t="inlineStr">
+      <c r="B885" t="inlineStr"/>
+      <c r="C885" t="inlineStr">
         <is>
           <t>挨拶 ,文字</t>
         </is>
       </c>
     </row>
-    <row r="887">
-      <c r="A887" t="inlineStr">
+    <row r="886">
+      <c r="A886" t="inlineStr">
         <is>
           <t xml:space="preserve">「昼寝の時間だ」
 إنه وقت القيلولة
@@ -16094,22 +16077,22 @@
 2501 https://x.com/NatGeoMagArab/status/1858049951579910486 </t>
         </is>
       </c>
-      <c r="B887" t="inlineStr"/>
-      <c r="C887" t="inlineStr">
+      <c r="B886" t="inlineStr"/>
+      <c r="C886" t="inlineStr">
         <is>
           <t>手書き語学 ,アラビア語 ,ペンギン</t>
         </is>
       </c>
     </row>
-    <row r="888">
-      <c r="A888" t="inlineStr">
+    <row r="887">
+      <c r="A887" t="inlineStr">
         <is>
           <t xml:space="preserve">（コピー用
 0001 </t>
         </is>
       </c>
-      <c r="B888" t="inlineStr"/>
-      <c r="C888" t="inlineStr"/>
+      <c r="B887" t="inlineStr"/>
+      <c r="C887" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>